<commit_message>
arreglo de colocacion de espacio faltaria terminar el tema de contemplar del id operativo
</commit_message>
<xml_diff>
--- a/Planilla_informe.xlsx
+++ b/Planilla_informe.xlsx
@@ -13778,22 +13778,22 @@
       </c>
       <c r="C4" s="259" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 6619/2024</t>
+          <t>FCB-14275/2024</t>
         </is>
       </c>
       <c r="D4" s="260" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 6619/2024-(1)</t>
+          <t>FCB-14275/2024-(1)</t>
         </is>
       </c>
       <c r="E4" s="260" t="inlineStr">
         <is>
-          <t>USU</t>
+          <t>UC2</t>
         </is>
       </c>
       <c r="F4" s="260" t="inlineStr">
         <is>
-          <t>OTRO MANDATO JUDICIAL</t>
+          <t>ORDEN DE ALLANAMIENTO</t>
         </is>
       </c>
       <c r="G4" s="260" t="inlineStr">
@@ -13803,12 +13803,12 @@
       </c>
       <c r="H4" s="270" t="inlineStr">
         <is>
-          <t>TIERRA DEL FUEGO ANTARTIDA E ISLAS DEL ATLANTICO SUR</t>
+          <t>CORDOBA</t>
         </is>
       </c>
       <c r="I4" s="304" t="inlineStr">
         <is>
-          <t>USHUAIA</t>
+          <t>UC2</t>
         </is>
       </c>
       <c r="J4" s="272" t="inlineStr">
@@ -13818,7 +13818,7 @@
       </c>
       <c r="K4" s="272" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ALVEAR 158, CORDOBA - nan</t>
         </is>
       </c>
       <c r="L4" s="265" t="inlineStr">
@@ -13832,14 +13832,14 @@
         </is>
       </c>
       <c r="N4" s="266" t="n">
-        <v>-54.8422</v>
+        <v>-31.415165</v>
       </c>
       <c r="O4" s="267" t="n">
-        <v>-68.309703</v>
+        <v>-64.18058600000001</v>
       </c>
       <c r="P4" s="288" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="Q4" s="268" t="inlineStr">
@@ -13871,22 +13871,22 @@
       </c>
       <c r="C5" s="259" t="inlineStr">
         <is>
-          <t>FCB 14275/2024</t>
+          <t>FCB-14275/2024</t>
         </is>
       </c>
       <c r="D5" s="260" t="inlineStr">
         <is>
-          <t>FCB 14275/2024-(1)</t>
+          <t>FCB-14275/2024-(2)</t>
         </is>
       </c>
       <c r="E5" s="260" t="inlineStr">
         <is>
-          <t>UC2</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="F5" s="260" t="inlineStr">
         <is>
-          <t>ORDEN DE ALLANAMIENTO</t>
+          <t>OTRO MANDATO JUDICIAL</t>
         </is>
       </c>
       <c r="G5" s="260" t="inlineStr">
@@ -13901,7 +13901,7 @@
       </c>
       <c r="I5" s="306" t="inlineStr">
         <is>
-          <t>UC2</t>
+          <t>CAPITAL</t>
         </is>
       </c>
       <c r="J5" s="272" t="inlineStr">
@@ -13911,7 +13911,7 @@
       </c>
       <c r="K5" s="272" t="inlineStr">
         <is>
-          <t>ALVEAR 158, CORDOBA - nan</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L5" s="265" t="inlineStr">
@@ -13925,10 +13925,10 @@
         </is>
       </c>
       <c r="N5" s="266" t="n">
-        <v>-31.415165</v>
+        <v>-31.314897</v>
       </c>
       <c r="O5" s="267" t="n">
-        <v>-64.18058600000001</v>
+        <v>-64.213159</v>
       </c>
       <c r="P5" s="288" t="inlineStr">
         <is>
@@ -13937,7 +13937,7 @@
       </c>
       <c r="Q5" s="268" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="R5" s="226" t="inlineStr">
@@ -13964,37 +13964,37 @@
       </c>
       <c r="C6" s="277" t="inlineStr">
         <is>
-          <t>FCB14275/2024</t>
+          <t>PS-0565-AER/24</t>
         </is>
       </c>
       <c r="D6" s="271" t="inlineStr">
         <is>
-          <t>FCB14275/2024-(1)</t>
+          <t>PS-0565-AER/24-(2)</t>
         </is>
       </c>
       <c r="E6" s="272" t="inlineStr">
         <is>
-          <t>COR</t>
+          <t>AER</t>
         </is>
       </c>
       <c r="F6" s="272" t="inlineStr">
         <is>
-          <t>OTRO MANDATO JUDICIAL</t>
+          <t>DENUNCIA POLICIAL</t>
         </is>
       </c>
       <c r="G6" s="272" t="inlineStr">
         <is>
-          <t>ORDEN JUDICIAL</t>
+          <t>ORDEN POLICIAL</t>
         </is>
       </c>
       <c r="H6" s="272" t="inlineStr">
         <is>
-          <t>CORDOBA</t>
+          <t>CIUDAD AUTONOMA DE BUENOS AIRES</t>
         </is>
       </c>
       <c r="I6" s="307" t="inlineStr">
         <is>
-          <t>CAPITAL</t>
+          <t>COMUNA 14</t>
         </is>
       </c>
       <c r="J6" s="269" t="inlineStr">
@@ -14004,7 +14004,7 @@
       </c>
       <c r="K6" s="271" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>nan nan, nan - nan</t>
         </is>
       </c>
       <c r="L6" s="265" t="inlineStr">
@@ -14018,10 +14018,10 @@
         </is>
       </c>
       <c r="N6" s="281" t="n">
-        <v>-31.314897</v>
+        <v>-34.55602</v>
       </c>
       <c r="O6" s="283" t="n">
-        <v>-64.213159</v>
+        <v>-58.41298</v>
       </c>
       <c r="P6" s="284" t="inlineStr">
         <is>
@@ -14030,7 +14030,7 @@
       </c>
       <c r="Q6" s="286" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="R6" s="274" t="inlineStr">
@@ -14057,12 +14057,12 @@
       </c>
       <c r="C7" s="277" t="inlineStr">
         <is>
-          <t>PS-0565-AER/24</t>
+          <t>PS-0575-AER/24</t>
         </is>
       </c>
       <c r="D7" s="272" t="inlineStr">
         <is>
-          <t>PS-0565-AER/24-(2)</t>
+          <t>PS-0575-AER/24-(2)</t>
         </is>
       </c>
       <c r="E7" s="272" t="inlineStr">
@@ -14097,7 +14097,7 @@
       </c>
       <c r="K7" s="272" t="inlineStr">
         <is>
-          <t>nan nan, nan - nan</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L7" s="265" t="inlineStr">
@@ -14111,19 +14111,19 @@
         </is>
       </c>
       <c r="N7" s="280" t="n">
-        <v>-34.55602</v>
+        <v>-34.5580305</v>
       </c>
       <c r="O7" s="282" t="n">
-        <v>-58.41298</v>
+        <v>-58.4191975</v>
       </c>
       <c r="P7" s="284" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>13/10/2024</t>
         </is>
       </c>
       <c r="Q7" s="286" t="inlineStr">
         <is>
-          <t>22:20</t>
+          <t>05:30</t>
         </is>
       </c>
       <c r="R7" s="274" t="inlineStr">
@@ -14150,17 +14150,17 @@
       </c>
       <c r="C8" s="277" t="inlineStr">
         <is>
-          <t>FGR 5144/2024</t>
+          <t>ACTUACIONES JUDICIALES-0000-UC1/24</t>
         </is>
       </c>
       <c r="D8" s="272" t="inlineStr">
         <is>
-          <t>FGR 5144/2024-(1)</t>
+          <t>ACTUACIONES JUDICIALES-0000-UC1/24-(1)</t>
         </is>
       </c>
       <c r="E8" s="272" t="inlineStr">
         <is>
-          <t>UC5</t>
+          <t>UC1</t>
         </is>
       </c>
       <c r="F8" s="272" t="inlineStr">
@@ -14175,12 +14175,12 @@
       </c>
       <c r="H8" s="272" t="inlineStr">
         <is>
-          <t>RIO NEGRO</t>
+          <t>CIUDAD AUTONOMA DE BUENOS AIRES</t>
         </is>
       </c>
       <c r="I8" s="307" t="inlineStr">
         <is>
-          <t>UC5</t>
+          <t>UC1</t>
         </is>
       </c>
       <c r="J8" s="272" t="inlineStr">
@@ -14190,7 +14190,7 @@
       </c>
       <c r="K8" s="272" t="inlineStr">
         <is>
-          <t>nan 62, SAN CARLOS DE BARILOCHE - nan</t>
+          <t>GENERAL CESAR DIAZ 4342, nan - nan</t>
         </is>
       </c>
       <c r="L8" s="265" t="inlineStr">
@@ -14204,19 +14204,19 @@
         </is>
       </c>
       <c r="N8" s="280" t="n">
-        <v>-41.15278</v>
+        <v>-34.6242611</v>
       </c>
       <c r="O8" s="282" t="n">
-        <v>-71.28045</v>
+        <v>-58.4932984</v>
       </c>
       <c r="P8" s="284" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="Q8" s="286" t="inlineStr">
         <is>
-          <t>07:25</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="R8" s="274" t="inlineStr">
@@ -14243,37 +14243,37 @@
       </c>
       <c r="C9" s="277" t="inlineStr">
         <is>
-          <t>FGR 5144/2024</t>
+          <t>FCB-14653/24 COIRON-222549/24</t>
         </is>
       </c>
       <c r="D9" s="272" t="inlineStr">
         <is>
-          <t>FGR 5144/2024-(2)</t>
+          <t>FCB-14653/24 COIRON-222549/24-(1)</t>
         </is>
       </c>
       <c r="E9" s="272" t="inlineStr">
         <is>
-          <t>UC5</t>
+          <t>UC2</t>
         </is>
       </c>
       <c r="F9" s="272" t="inlineStr">
         <is>
-          <t>ORDEN DE ALLANAMIENTO</t>
+          <t>DENUNCIA POLICIAL</t>
         </is>
       </c>
       <c r="G9" s="272" t="inlineStr">
         <is>
-          <t>ORDEN JUDICIAL</t>
+          <t>ORDEN POLICIAL</t>
         </is>
       </c>
       <c r="H9" s="272" t="inlineStr">
         <is>
-          <t>RIO NEGRO</t>
+          <t>CORDOBA</t>
         </is>
       </c>
       <c r="I9" s="307" t="inlineStr">
         <is>
-          <t>UC5</t>
+          <t>UC2</t>
         </is>
       </c>
       <c r="J9" s="272" t="inlineStr">
@@ -14283,7 +14283,7 @@
       </c>
       <c r="K9" s="272" t="inlineStr">
         <is>
-          <t>ÑANCU LAHUEN 313, SAN CARLOS DE BARILOCHE - nan</t>
+          <t>EDUARDO MARQUINA S/D, CORDOBA - nan</t>
         </is>
       </c>
       <c r="L9" s="265" t="inlineStr">
@@ -14297,19 +14297,19 @@
         </is>
       </c>
       <c r="N9" s="280" t="n">
-        <v>-41.16245</v>
+        <v>-31.381514</v>
       </c>
       <c r="O9" s="282" t="n">
-        <v>-71.32853</v>
+        <v>-64.192876</v>
       </c>
       <c r="P9" s="284" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="Q9" s="286" t="inlineStr">
         <is>
-          <t>07:30</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="R9" s="274" t="inlineStr">
@@ -14336,37 +14336,37 @@
       </c>
       <c r="C10" s="277" t="inlineStr">
         <is>
-          <t xml:space="preserve"> FCR 10153/2023</t>
+          <t>179/2023 (8178)</t>
         </is>
       </c>
       <c r="D10" s="272" t="inlineStr">
         <is>
-          <t xml:space="preserve"> FCR 10153/2023-(1)</t>
+          <t>179/2023 (8178)-(1)</t>
         </is>
       </c>
       <c r="E10" s="272" t="inlineStr">
         <is>
-          <t>PMY</t>
+          <t>AER</t>
         </is>
       </c>
       <c r="F10" s="272" t="inlineStr">
         <is>
-          <t>OTRO MANDATO JUDICIAL</t>
+          <t>DENUNCIA POLICIAL</t>
         </is>
       </c>
       <c r="G10" s="272" t="inlineStr">
         <is>
-          <t>ORDEN JUDICIAL</t>
+          <t>ORDEN POLICIAL</t>
         </is>
       </c>
       <c r="H10" s="272" t="inlineStr">
         <is>
-          <t>CHUBUT</t>
+          <t>CIUDAD AUTONOMA DE BUENOS AIRES</t>
         </is>
       </c>
       <c r="I10" s="307" t="inlineStr">
         <is>
-          <t>BIEDMA</t>
+          <t>COMUNA 14</t>
         </is>
       </c>
       <c r="J10" s="272" t="inlineStr">
@@ -14390,19 +14390,19 @@
         </is>
       </c>
       <c r="N10" s="278" t="n">
-        <v>-42.754988</v>
+        <v>-34.5580305</v>
       </c>
       <c r="O10" s="282" t="n">
-        <v>-65.10066500000001</v>
+        <v>-58.4191975</v>
       </c>
       <c r="P10" s="284" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="Q10" s="286" t="inlineStr">
         <is>
-          <t>23:10</t>
+          <t>08:20</t>
         </is>
       </c>
       <c r="R10" s="274" t="inlineStr">
@@ -14429,17 +14429,17 @@
       </c>
       <c r="C11" s="277" t="inlineStr">
         <is>
-          <t>FCR  8591/2024</t>
+          <t>42933 "M" 2021</t>
         </is>
       </c>
       <c r="D11" s="269" t="inlineStr">
         <is>
-          <t>FCR  8591/2024-(1)</t>
+          <t>42933 "M" 2021-(1)</t>
         </is>
       </c>
       <c r="E11" s="269" t="inlineStr">
         <is>
-          <t>CAL</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="F11" s="269" t="inlineStr">
@@ -14454,12 +14454,12 @@
       </c>
       <c r="H11" s="272" t="inlineStr">
         <is>
-          <t>SANTA CRUZ</t>
+          <t>CORDOBA</t>
         </is>
       </c>
       <c r="I11" s="307" t="inlineStr">
         <is>
-          <t>LAGO ARGENTINO</t>
+          <t>CAPITAL</t>
         </is>
       </c>
       <c r="J11" s="272" t="inlineStr">
@@ -14483,19 +14483,19 @@
         </is>
       </c>
       <c r="N11" s="279" t="n">
-        <v>-50.283977</v>
+        <v>-31.315538</v>
       </c>
       <c r="O11" s="279" t="n">
-        <v>-72.053724</v>
+        <v>-64.213374</v>
       </c>
       <c r="P11" s="284" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="Q11" s="287" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>03:30</t>
         </is>
       </c>
       <c r="R11" s="274" t="inlineStr">
@@ -14522,37 +14522,37 @@
       </c>
       <c r="C12" s="277" t="inlineStr">
         <is>
-          <t>PS-0575-AER/24</t>
+          <t>27091/2022</t>
         </is>
       </c>
       <c r="D12" s="272" t="inlineStr">
         <is>
-          <t>PS-0575-AER/24-(2)</t>
+          <t>27091/2022-(1)</t>
         </is>
       </c>
       <c r="E12" s="272" t="inlineStr">
         <is>
-          <t>AER</t>
+          <t>UCC</t>
         </is>
       </c>
       <c r="F12" s="269" t="inlineStr">
         <is>
-          <t>DENUNCIA POLICIAL</t>
+          <t>ORDEN DE ALLANAMIENTO</t>
         </is>
       </c>
       <c r="G12" s="269" t="inlineStr">
         <is>
-          <t>ORDEN POLICIAL</t>
+          <t>ORDEN JUDICIAL</t>
         </is>
       </c>
       <c r="H12" s="272" t="inlineStr">
         <is>
-          <t>CIUDAD AUTONOMA DE BUENOS AIRES</t>
+          <t>BUENOS AIRES</t>
         </is>
       </c>
       <c r="I12" s="307" t="inlineStr">
         <is>
-          <t>COMUNA 14</t>
+          <t>UCC</t>
         </is>
       </c>
       <c r="J12" s="272" t="inlineStr">
@@ -14562,7 +14562,7 @@
       </c>
       <c r="K12" s="276" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>VILLEGAS 149, EL PALOMAR - MORON</t>
         </is>
       </c>
       <c r="L12" s="265" t="inlineStr">
@@ -14576,19 +14576,19 @@
         </is>
       </c>
       <c r="N12" s="264" t="n">
-        <v>-34.5580305</v>
+        <v>-34.623564</v>
       </c>
       <c r="O12" s="262" t="n">
-        <v>-58.4191975</v>
+        <v>-58.577936</v>
       </c>
       <c r="P12" s="263" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="Q12" s="285" t="inlineStr">
         <is>
-          <t>05:30</t>
+          <t>07:57</t>
         </is>
       </c>
       <c r="R12" s="274" t="inlineStr">
@@ -14615,22 +14615,22 @@
       </c>
       <c r="C13" s="277" t="inlineStr">
         <is>
-          <t>FGR5144/2024</t>
+          <t>27091/2022</t>
         </is>
       </c>
       <c r="D13" s="271" t="inlineStr">
         <is>
-          <t>FGR5144/2024-(1)</t>
+          <t>27091/2022-(2)</t>
         </is>
       </c>
       <c r="E13" s="272" t="inlineStr">
         <is>
-          <t>UC5</t>
+          <t>UCC</t>
         </is>
       </c>
       <c r="F13" s="272" t="inlineStr">
         <is>
-          <t>OTRO MANDATO JUDICIAL</t>
+          <t>ORDEN DE ALLANAMIENTO</t>
         </is>
       </c>
       <c r="G13" s="272" t="inlineStr">
@@ -14640,12 +14640,12 @@
       </c>
       <c r="H13" s="272" t="inlineStr">
         <is>
-          <t>RIO NEGRO</t>
+          <t>BUENOS AIRES</t>
         </is>
       </c>
       <c r="I13" s="307" t="inlineStr">
         <is>
-          <t>UC5</t>
+          <t>UCC</t>
         </is>
       </c>
       <c r="J13" s="269" t="inlineStr">
@@ -14655,7 +14655,7 @@
       </c>
       <c r="K13" s="271" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>BELGRANO 6564, JOSE LEON SUAREZ - SAN MARTIN</t>
         </is>
       </c>
       <c r="L13" s="265" t="inlineStr">
@@ -14669,19 +14669,19 @@
         </is>
       </c>
       <c r="N13" s="281" t="n">
-        <v>-41.146694</v>
+        <v>-34.541669</v>
       </c>
       <c r="O13" s="283" t="n">
-        <v>-71.16198199999999</v>
+        <v>-58.574293</v>
       </c>
       <c r="P13" s="263" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="Q13" s="286" t="inlineStr">
         <is>
-          <t>11:20</t>
+          <t>07:40</t>
         </is>
       </c>
       <c r="R13" s="274" t="inlineStr">
@@ -14701,746 +14701,178 @@
       <c r="Z13" s="305" t="n"/>
     </row>
     <row r="14" ht="18.75" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B14" s="270" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C14" s="277" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 21300/17-V</t>
-        </is>
-      </c>
-      <c r="D14" s="271" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 21300/17-V-(1)</t>
-        </is>
-      </c>
-      <c r="E14" s="272" t="inlineStr">
-        <is>
-          <t>CRV</t>
-        </is>
-      </c>
-      <c r="F14" s="272" t="inlineStr">
-        <is>
-          <t>CONTROL PREVENTIVO - SECTOR DE SEGURIDAD RESTRINGIDA AEROPORTUARIA</t>
-        </is>
-      </c>
-      <c r="G14" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN POLICIAL</t>
-        </is>
-      </c>
-      <c r="H14" s="272" t="inlineStr">
-        <is>
-          <t>CHUBUT</t>
-        </is>
-      </c>
-      <c r="I14" s="307" t="inlineStr">
-        <is>
-          <t>ESCALANTE</t>
-        </is>
-      </c>
-      <c r="J14" s="269" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K14" s="271" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L14" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M14" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N14" s="281" t="n">
-        <v>-45.789465</v>
-      </c>
-      <c r="O14" s="283" t="n">
-        <v>-67.467674</v>
-      </c>
-      <c r="P14" s="263" t="inlineStr">
-        <is>
-          <t>16/10/2024</t>
-        </is>
-      </c>
-      <c r="Q14" s="286" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="R14" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S14" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T14" t="n">
-        <v/>
-      </c>
+      <c r="B14" s="270" t="n"/>
+      <c r="C14" s="277" t="n"/>
+      <c r="D14" s="271" t="n"/>
+      <c r="E14" s="272" t="n"/>
+      <c r="F14" s="272" t="n"/>
+      <c r="G14" s="272" t="n"/>
+      <c r="H14" s="272" t="n"/>
+      <c r="I14" s="307" t="n"/>
+      <c r="J14" s="269" t="n"/>
+      <c r="K14" s="271" t="n"/>
+      <c r="L14" s="265" t="n"/>
+      <c r="M14" s="265" t="n"/>
+      <c r="N14" s="281" t="n"/>
+      <c r="O14" s="283" t="n"/>
+      <c r="P14" s="263" t="n"/>
+      <c r="Q14" s="286" t="n"/>
+      <c r="R14" s="274" t="n"/>
+      <c r="S14" s="275" t="n"/>
       <c r="Y14" s="305" t="n"/>
       <c r="Z14" s="305" t="n"/>
     </row>
     <row r="15" ht="16.5" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B15" s="270" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C15" s="277" t="inlineStr">
-        <is>
-          <t>FCB 14653/24 COIRON 222549/24</t>
-        </is>
-      </c>
-      <c r="D15" s="271" t="inlineStr">
-        <is>
-          <t>FCB 14653/24 COIRON 222549/24-(1)</t>
-        </is>
-      </c>
-      <c r="E15" s="272" t="inlineStr">
-        <is>
-          <t>UC2</t>
-        </is>
-      </c>
-      <c r="F15" s="272" t="inlineStr">
-        <is>
-          <t>DENUNCIA POLICIAL</t>
-        </is>
-      </c>
-      <c r="G15" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN POLICIAL</t>
-        </is>
-      </c>
-      <c r="H15" s="272" t="inlineStr">
-        <is>
-          <t>CORDOBA</t>
-        </is>
-      </c>
-      <c r="I15" s="307" t="inlineStr">
-        <is>
-          <t>UC2</t>
-        </is>
-      </c>
-      <c r="J15" s="269" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K15" s="271" t="inlineStr">
-        <is>
-          <t>EDUARDO MARQUINA S/D, CORDOBA - nan</t>
-        </is>
-      </c>
-      <c r="L15" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M15" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N15" s="281" t="n">
-        <v>-31.381514</v>
-      </c>
-      <c r="O15" s="283" t="n">
-        <v>-64.192876</v>
-      </c>
-      <c r="P15" s="263" t="inlineStr">
-        <is>
-          <t>14/10/2024</t>
-        </is>
-      </c>
-      <c r="Q15" s="286" t="inlineStr">
-        <is>
-          <t>12:36</t>
-        </is>
-      </c>
-      <c r="R15" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S15" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T15" t="n">
-        <v/>
-      </c>
+      <c r="B15" s="270" t="n"/>
+      <c r="C15" s="277" t="n"/>
+      <c r="D15" s="271" t="n"/>
+      <c r="E15" s="272" t="n"/>
+      <c r="F15" s="272" t="n"/>
+      <c r="G15" s="272" t="n"/>
+      <c r="H15" s="272" t="n"/>
+      <c r="I15" s="307" t="n"/>
+      <c r="J15" s="269" t="n"/>
+      <c r="K15" s="271" t="n"/>
+      <c r="L15" s="265" t="n"/>
+      <c r="M15" s="265" t="n"/>
+      <c r="N15" s="281" t="n"/>
+      <c r="O15" s="283" t="n"/>
+      <c r="P15" s="263" t="n"/>
+      <c r="Q15" s="286" t="n"/>
+      <c r="R15" s="274" t="n"/>
+      <c r="S15" s="275" t="n"/>
       <c r="Y15" s="305" t="n"/>
       <c r="Z15" s="305" t="n"/>
     </row>
     <row r="16" ht="19.5" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B16" s="270" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C16" s="277" t="inlineStr">
-        <is>
-          <t>CARPETA-N 9700</t>
-        </is>
-      </c>
-      <c r="D16" s="271" t="inlineStr">
-        <is>
-          <t>CARPETA-N 9700-(1)</t>
-        </is>
-      </c>
-      <c r="E16" s="272" t="inlineStr">
-        <is>
-          <t>TRE</t>
-        </is>
-      </c>
-      <c r="F16" s="272" t="inlineStr">
-        <is>
-          <t>CONTROL PREVENTIVO - DESPLIEGUE</t>
-        </is>
-      </c>
-      <c r="G16" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN POLICIAL</t>
-        </is>
-      </c>
-      <c r="H16" s="272" t="inlineStr">
-        <is>
-          <t>CHUBUT</t>
-        </is>
-      </c>
-      <c r="I16" s="307" t="inlineStr">
-        <is>
-          <t>RAWSON</t>
-        </is>
-      </c>
-      <c r="J16" s="269" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K16" s="271" t="inlineStr">
-        <is>
-          <t>nan nan, TRELEW - nan</t>
-        </is>
-      </c>
-      <c r="L16" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M16" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N16" s="281" t="n">
-        <v>-43.24824</v>
-      </c>
-      <c r="O16" s="283" t="n">
-        <v>-65.30496100000001</v>
-      </c>
-      <c r="P16" s="263" t="inlineStr">
-        <is>
-          <t>18/10/2024</t>
-        </is>
-      </c>
-      <c r="Q16" s="286" t="inlineStr">
-        <is>
-          <t>18:30</t>
-        </is>
-      </c>
-      <c r="R16" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S16" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T16" t="n">
-        <v/>
-      </c>
+      <c r="B16" s="270" t="n"/>
+      <c r="C16" s="277" t="n"/>
+      <c r="D16" s="271" t="n"/>
+      <c r="E16" s="272" t="n"/>
+      <c r="F16" s="272" t="n"/>
+      <c r="G16" s="272" t="n"/>
+      <c r="H16" s="272" t="n"/>
+      <c r="I16" s="307" t="n"/>
+      <c r="J16" s="269" t="n"/>
+      <c r="K16" s="271" t="n"/>
+      <c r="L16" s="265" t="n"/>
+      <c r="M16" s="265" t="n"/>
+      <c r="N16" s="281" t="n"/>
+      <c r="O16" s="283" t="n"/>
+      <c r="P16" s="263" t="n"/>
+      <c r="Q16" s="286" t="n"/>
+      <c r="R16" s="274" t="n"/>
+      <c r="S16" s="275" t="n"/>
       <c r="Y16" s="305" t="n"/>
       <c r="Z16" s="305" t="n"/>
     </row>
     <row r="17" ht="18" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B17" s="277" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C17" s="277" t="inlineStr">
-        <is>
-          <t>179/2023 (8178)</t>
-        </is>
-      </c>
-      <c r="D17" s="272" t="inlineStr">
-        <is>
-          <t>179/2023 (8178)-(1)</t>
-        </is>
-      </c>
-      <c r="E17" s="272" t="inlineStr">
-        <is>
-          <t>AER</t>
-        </is>
-      </c>
-      <c r="F17" s="272" t="inlineStr">
-        <is>
-          <t>DENUNCIA POLICIAL</t>
-        </is>
-      </c>
-      <c r="G17" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN POLICIAL</t>
-        </is>
-      </c>
-      <c r="H17" s="272" t="inlineStr">
-        <is>
-          <t>CIUDAD AUTONOMA DE BUENOS AIRES</t>
-        </is>
-      </c>
-      <c r="I17" s="307" t="inlineStr">
-        <is>
-          <t>COMUNA 14</t>
-        </is>
-      </c>
-      <c r="J17" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K17" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L17" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M17" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N17" s="280" t="n">
-        <v>-34.5580305</v>
-      </c>
-      <c r="O17" s="282" t="n">
-        <v>-58.4191975</v>
-      </c>
-      <c r="P17" s="263" t="inlineStr">
-        <is>
-          <t>19/10/2024</t>
-        </is>
-      </c>
-      <c r="Q17" s="286" t="inlineStr">
-        <is>
-          <t>08:20</t>
-        </is>
-      </c>
-      <c r="R17" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S17" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T17" t="n">
-        <v/>
-      </c>
+      <c r="B17" s="277" t="n"/>
+      <c r="C17" s="277" t="n"/>
+      <c r="D17" s="272" t="n"/>
+      <c r="E17" s="272" t="n"/>
+      <c r="F17" s="272" t="n"/>
+      <c r="G17" s="272" t="n"/>
+      <c r="H17" s="272" t="n"/>
+      <c r="I17" s="307" t="n"/>
+      <c r="J17" s="272" t="n"/>
+      <c r="K17" s="272" t="n"/>
+      <c r="L17" s="265" t="n"/>
+      <c r="M17" s="265" t="n"/>
+      <c r="N17" s="280" t="n"/>
+      <c r="O17" s="282" t="n"/>
+      <c r="P17" s="263" t="n"/>
+      <c r="Q17" s="286" t="n"/>
+      <c r="R17" s="274" t="n"/>
+      <c r="S17" s="275" t="n"/>
       <c r="Y17" s="305" t="n"/>
       <c r="Z17" s="305" t="n"/>
     </row>
     <row r="18" ht="19.5" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B18" s="277" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C18" s="277" t="inlineStr">
-        <is>
-          <t>42933 "M" 2021</t>
-        </is>
-      </c>
-      <c r="D18" s="272" t="inlineStr">
-        <is>
-          <t>42933 "M" 2021-(1)</t>
-        </is>
-      </c>
-      <c r="E18" s="272" t="inlineStr">
-        <is>
-          <t>COR</t>
-        </is>
-      </c>
-      <c r="F18" s="272" t="inlineStr">
-        <is>
-          <t>DENUNCIA POLICIAL</t>
-        </is>
-      </c>
-      <c r="G18" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN POLICIAL</t>
-        </is>
-      </c>
-      <c r="H18" s="272" t="inlineStr">
-        <is>
-          <t>CORDOBA</t>
-        </is>
-      </c>
-      <c r="I18" s="307" t="inlineStr">
-        <is>
-          <t>CAPITAL</t>
-        </is>
-      </c>
-      <c r="J18" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K18" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L18" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M18" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N18" s="280" t="n">
-        <v>-31.315538</v>
-      </c>
-      <c r="O18" s="282" t="n">
-        <v>-64.213374</v>
-      </c>
-      <c r="P18" s="263" t="inlineStr">
-        <is>
-          <t>20/10/2024</t>
-        </is>
-      </c>
-      <c r="Q18" s="286" t="inlineStr">
-        <is>
-          <t>03:30</t>
-        </is>
-      </c>
-      <c r="R18" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S18" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T18" t="n">
-        <v/>
-      </c>
+      <c r="B18" s="277" t="n"/>
+      <c r="C18" s="277" t="n"/>
+      <c r="D18" s="272" t="n"/>
+      <c r="E18" s="272" t="n"/>
+      <c r="F18" s="272" t="n"/>
+      <c r="G18" s="272" t="n"/>
+      <c r="H18" s="272" t="n"/>
+      <c r="I18" s="307" t="n"/>
+      <c r="J18" s="272" t="n"/>
+      <c r="K18" s="272" t="n"/>
+      <c r="L18" s="265" t="n"/>
+      <c r="M18" s="265" t="n"/>
+      <c r="N18" s="280" t="n"/>
+      <c r="O18" s="282" t="n"/>
+      <c r="P18" s="263" t="n"/>
+      <c r="Q18" s="286" t="n"/>
+      <c r="R18" s="274" t="n"/>
+      <c r="S18" s="275" t="n"/>
       <c r="Y18" s="305" t="n"/>
       <c r="Z18" s="305" t="n"/>
     </row>
     <row r="19" ht="21" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B19" s="277" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C19" s="277" t="inlineStr">
-        <is>
-          <t>LEG CONTRAVENCIONAL 1762</t>
-        </is>
-      </c>
-      <c r="D19" s="272" t="inlineStr">
-        <is>
-          <t>LEG CONTRAVENCIONAL 1762-(1)</t>
-        </is>
-      </c>
-      <c r="E19" s="272" t="inlineStr">
-        <is>
-          <t>CRV</t>
-        </is>
-      </c>
-      <c r="F19" s="272" t="inlineStr">
-        <is>
-          <t>CONTROL PREVENTIVO - SECTOR DE SEGURIDAD RESTRINGIDA AEROPORTUARIA</t>
-        </is>
-      </c>
-      <c r="G19" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN POLICIAL</t>
-        </is>
-      </c>
-      <c r="H19" s="272" t="inlineStr">
-        <is>
-          <t>CHUBUT</t>
-        </is>
-      </c>
-      <c r="I19" s="307" t="inlineStr">
-        <is>
-          <t>ESCALANTE</t>
-        </is>
-      </c>
-      <c r="J19" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K19" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L19" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M19" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N19" s="280" t="n">
-        <v>-45.789465</v>
-      </c>
-      <c r="O19" s="282" t="n">
-        <v>-67.467674</v>
-      </c>
-      <c r="P19" s="263" t="inlineStr">
-        <is>
-          <t>21/10/2024</t>
-        </is>
-      </c>
-      <c r="Q19" s="286" t="inlineStr">
-        <is>
-          <t>21:00</t>
-        </is>
-      </c>
-      <c r="R19" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S19" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T19" t="n">
-        <v/>
-      </c>
+      <c r="B19" s="277" t="n"/>
+      <c r="C19" s="277" t="n"/>
+      <c r="D19" s="272" t="n"/>
+      <c r="E19" s="272" t="n"/>
+      <c r="F19" s="272" t="n"/>
+      <c r="G19" s="272" t="n"/>
+      <c r="H19" s="272" t="n"/>
+      <c r="I19" s="307" t="n"/>
+      <c r="J19" s="272" t="n"/>
+      <c r="K19" s="272" t="n"/>
+      <c r="L19" s="265" t="n"/>
+      <c r="M19" s="265" t="n"/>
+      <c r="N19" s="280" t="n"/>
+      <c r="O19" s="282" t="n"/>
+      <c r="P19" s="263" t="n"/>
+      <c r="Q19" s="286" t="n"/>
+      <c r="R19" s="274" t="n"/>
+      <c r="S19" s="275" t="n"/>
       <c r="Y19" s="305" t="n"/>
       <c r="Z19" s="305" t="n"/>
     </row>
     <row r="20" ht="20.25" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B20" s="277" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C20" s="277" t="inlineStr">
-        <is>
-          <t>27091/2022</t>
-        </is>
-      </c>
-      <c r="D20" s="272" t="inlineStr">
-        <is>
-          <t>27091/2022-(1)</t>
-        </is>
-      </c>
-      <c r="E20" s="272" t="inlineStr">
-        <is>
-          <t>UCC</t>
-        </is>
-      </c>
-      <c r="F20" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN DE ALLANAMIENTO</t>
-        </is>
-      </c>
-      <c r="G20" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN JUDICIAL</t>
-        </is>
-      </c>
-      <c r="H20" s="272" t="inlineStr">
-        <is>
-          <t>BUENOS AIRES</t>
-        </is>
-      </c>
-      <c r="I20" s="307" t="inlineStr">
-        <is>
-          <t>UCC</t>
-        </is>
-      </c>
-      <c r="J20" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K20" s="272" t="inlineStr">
-        <is>
-          <t>VILLEGAS 149, EL PALOMAR - MORON</t>
-        </is>
-      </c>
-      <c r="L20" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M20" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N20" s="278" t="n">
-        <v>-34.623564</v>
-      </c>
-      <c r="O20" s="282" t="n">
-        <v>-58.577936</v>
-      </c>
-      <c r="P20" s="263" t="inlineStr">
-        <is>
-          <t>22/10/2024</t>
-        </is>
-      </c>
-      <c r="Q20" s="286" t="inlineStr">
-        <is>
-          <t>07:57</t>
-        </is>
-      </c>
-      <c r="R20" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S20" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T20" t="n">
-        <v/>
-      </c>
+      <c r="B20" s="277" t="n"/>
+      <c r="C20" s="277" t="n"/>
+      <c r="D20" s="272" t="n"/>
+      <c r="E20" s="272" t="n"/>
+      <c r="F20" s="272" t="n"/>
+      <c r="G20" s="272" t="n"/>
+      <c r="H20" s="272" t="n"/>
+      <c r="I20" s="307" t="n"/>
+      <c r="J20" s="272" t="n"/>
+      <c r="K20" s="272" t="n"/>
+      <c r="L20" s="265" t="n"/>
+      <c r="M20" s="265" t="n"/>
+      <c r="N20" s="278" t="n"/>
+      <c r="O20" s="282" t="n"/>
+      <c r="P20" s="263" t="n"/>
+      <c r="Q20" s="286" t="n"/>
+      <c r="R20" s="274" t="n"/>
+      <c r="S20" s="275" t="n"/>
       <c r="Y20" s="305" t="n"/>
       <c r="Z20" s="305" t="n"/>
     </row>
     <row r="21" ht="20.25" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B21" s="277" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C21" s="277" t="inlineStr">
-        <is>
-          <t>27091/2022</t>
-        </is>
-      </c>
-      <c r="D21" s="269" t="inlineStr">
-        <is>
-          <t>27091/2022-(2)</t>
-        </is>
-      </c>
-      <c r="E21" s="269" t="inlineStr">
-        <is>
-          <t>UCC</t>
-        </is>
-      </c>
-      <c r="F21" s="269" t="inlineStr">
-        <is>
-          <t>ORDEN DE ALLANAMIENTO</t>
-        </is>
-      </c>
-      <c r="G21" s="269" t="inlineStr">
-        <is>
-          <t>ORDEN JUDICIAL</t>
-        </is>
-      </c>
-      <c r="H21" s="272" t="inlineStr">
-        <is>
-          <t>BUENOS AIRES</t>
-        </is>
-      </c>
-      <c r="I21" s="307" t="inlineStr">
-        <is>
-          <t>UCC</t>
-        </is>
-      </c>
-      <c r="J21" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K21" s="272" t="inlineStr">
-        <is>
-          <t>BELGRANO 6564, JOSE LEON SUAREZ - SAN MARTIN</t>
-        </is>
-      </c>
-      <c r="L21" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M21" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N21" s="279" t="n">
-        <v>-34.541669</v>
-      </c>
-      <c r="O21" s="279" t="n">
-        <v>-58.574293</v>
-      </c>
-      <c r="P21" s="263" t="inlineStr">
-        <is>
-          <t>22/10/2024</t>
-        </is>
-      </c>
-      <c r="Q21" s="287" t="inlineStr">
-        <is>
-          <t>07:40</t>
-        </is>
-      </c>
-      <c r="R21" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S21" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T21" t="n">
-        <v/>
-      </c>
+      <c r="B21" s="277" t="n"/>
+      <c r="C21" s="277" t="n"/>
+      <c r="D21" s="269" t="n"/>
+      <c r="E21" s="269" t="n"/>
+      <c r="F21" s="269" t="n"/>
+      <c r="G21" s="269" t="n"/>
+      <c r="H21" s="272" t="n"/>
+      <c r="I21" s="307" t="n"/>
+      <c r="J21" s="272" t="n"/>
+      <c r="K21" s="272" t="n"/>
+      <c r="L21" s="265" t="n"/>
+      <c r="M21" s="265" t="n"/>
+      <c r="N21" s="279" t="n"/>
+      <c r="O21" s="279" t="n"/>
+      <c r="P21" s="263" t="n"/>
+      <c r="Q21" s="287" t="n"/>
+      <c r="R21" s="274" t="n"/>
+      <c r="S21" s="275" t="n"/>
       <c r="Y21" s="305" t="n"/>
       <c r="Z21" s="305" t="n"/>
     </row>

</xml_diff>

<commit_message>
arreglo en la copia en el archivo base es decir armar base propia de como se van a estandarizar los datos , luego  hay que crear un codigo para sigipol con el parte y año para el tema de contemplar para sigipol y poder filtrar lo que se informo desde 2023 hasta la fecha luego , en opereaciones voy a tener que buscar la forma de crear un codigo para el tema de ver si ya se informaron maso menos lo tengo informado
</commit_message>
<xml_diff>
--- a/Planilla_informe.xlsx
+++ b/Planilla_informe.xlsx
@@ -13616,7 +13616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -13771,932 +13771,222 @@
       </c>
     </row>
     <row r="4" ht="18.75" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B4" s="259" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C4" s="259" t="inlineStr">
-        <is>
-          <t>FCB-14275/2024</t>
-        </is>
-      </c>
-      <c r="D4" s="260" t="inlineStr">
-        <is>
-          <t>FCB-14275/2024-(1)</t>
-        </is>
-      </c>
-      <c r="E4" s="260" t="inlineStr">
-        <is>
-          <t>UC2</t>
-        </is>
-      </c>
-      <c r="F4" s="260" t="inlineStr">
-        <is>
-          <t>ORDEN DE ALLANAMIENTO</t>
-        </is>
-      </c>
-      <c r="G4" s="260" t="inlineStr">
-        <is>
-          <t>ORDEN JUDICIAL</t>
-        </is>
-      </c>
-      <c r="H4" s="270" t="inlineStr">
-        <is>
-          <t>CORDOBA</t>
-        </is>
-      </c>
-      <c r="I4" s="304" t="inlineStr">
-        <is>
-          <t>UC2</t>
-        </is>
-      </c>
-      <c r="J4" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K4" s="272" t="inlineStr">
-        <is>
-          <t>ALVEAR 158, CORDOBA - nan</t>
-        </is>
-      </c>
-      <c r="L4" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M4" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N4" s="266" t="n">
-        <v>-31.415165</v>
-      </c>
-      <c r="O4" s="267" t="n">
-        <v>-64.18058600000001</v>
-      </c>
-      <c r="P4" s="288" t="inlineStr">
-        <is>
-          <t>07/10/2024</t>
-        </is>
-      </c>
-      <c r="Q4" s="268" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
-      <c r="R4" s="226" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S4" s="227" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T4" t="n">
-        <v/>
-      </c>
+      <c r="B4" s="259" t="n"/>
+      <c r="C4" s="259" t="n"/>
+      <c r="D4" s="260" t="n"/>
+      <c r="E4" s="260" t="n"/>
+      <c r="F4" s="260" t="n"/>
+      <c r="G4" s="260" t="n"/>
+      <c r="H4" s="270" t="n"/>
+      <c r="I4" s="304" t="n"/>
+      <c r="J4" s="272" t="n"/>
+      <c r="K4" s="272" t="n"/>
+      <c r="L4" s="265" t="n"/>
+      <c r="M4" s="265" t="n"/>
+      <c r="N4" s="266" t="n"/>
+      <c r="O4" s="267" t="n"/>
+      <c r="P4" s="288" t="n"/>
+      <c r="Q4" s="268" t="n"/>
+      <c r="R4" s="226" t="n"/>
+      <c r="S4" s="227" t="n"/>
       <c r="Y4" s="305" t="n"/>
       <c r="Z4" s="305" t="n"/>
     </row>
     <row r="5" ht="18.75" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B5" s="259" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C5" s="259" t="inlineStr">
-        <is>
-          <t>FCB-14275/2024</t>
-        </is>
-      </c>
-      <c r="D5" s="260" t="inlineStr">
-        <is>
-          <t>FCB-14275/2024-(2)</t>
-        </is>
-      </c>
-      <c r="E5" s="260" t="inlineStr">
-        <is>
-          <t>COR</t>
-        </is>
-      </c>
-      <c r="F5" s="260" t="inlineStr">
-        <is>
-          <t>OTRO MANDATO JUDICIAL</t>
-        </is>
-      </c>
-      <c r="G5" s="260" t="inlineStr">
-        <is>
-          <t>ORDEN JUDICIAL</t>
-        </is>
-      </c>
-      <c r="H5" s="289" t="inlineStr">
-        <is>
-          <t>CORDOBA</t>
-        </is>
-      </c>
-      <c r="I5" s="306" t="inlineStr">
-        <is>
-          <t>CAPITAL</t>
-        </is>
-      </c>
-      <c r="J5" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K5" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L5" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M5" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N5" s="266" t="n">
-        <v>-31.314897</v>
-      </c>
-      <c r="O5" s="267" t="n">
-        <v>-64.213159</v>
-      </c>
-      <c r="P5" s="288" t="inlineStr">
-        <is>
-          <t>07/10/2024</t>
-        </is>
-      </c>
-      <c r="Q5" s="268" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
-      <c r="R5" s="226" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S5" s="227" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T5" t="n">
-        <v/>
-      </c>
+      <c r="B5" s="259" t="n"/>
+      <c r="C5" s="259" t="n"/>
+      <c r="D5" s="260" t="n"/>
+      <c r="E5" s="260" t="n"/>
+      <c r="F5" s="260" t="n"/>
+      <c r="G5" s="260" t="n"/>
+      <c r="H5" s="289" t="n"/>
+      <c r="I5" s="306" t="n"/>
+      <c r="J5" s="272" t="n"/>
+      <c r="K5" s="272" t="n"/>
+      <c r="L5" s="265" t="n"/>
+      <c r="M5" s="265" t="n"/>
+      <c r="N5" s="266" t="n"/>
+      <c r="O5" s="267" t="n"/>
+      <c r="P5" s="288" t="n"/>
+      <c r="Q5" s="268" t="n"/>
+      <c r="R5" s="226" t="n"/>
+      <c r="S5" s="227" t="n"/>
       <c r="Y5" s="305" t="n"/>
       <c r="Z5" s="305" t="n"/>
     </row>
     <row r="6" ht="18.75" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B6" s="270" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C6" s="277" t="inlineStr">
-        <is>
-          <t>PS-0565-AER/24</t>
-        </is>
-      </c>
-      <c r="D6" s="271" t="inlineStr">
-        <is>
-          <t>PS-0565-AER/24-(2)</t>
-        </is>
-      </c>
-      <c r="E6" s="272" t="inlineStr">
-        <is>
-          <t>AER</t>
-        </is>
-      </c>
-      <c r="F6" s="272" t="inlineStr">
-        <is>
-          <t>DENUNCIA POLICIAL</t>
-        </is>
-      </c>
-      <c r="G6" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN POLICIAL</t>
-        </is>
-      </c>
-      <c r="H6" s="272" t="inlineStr">
-        <is>
-          <t>CIUDAD AUTONOMA DE BUENOS AIRES</t>
-        </is>
-      </c>
-      <c r="I6" s="307" t="inlineStr">
-        <is>
-          <t>COMUNA 14</t>
-        </is>
-      </c>
-      <c r="J6" s="269" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K6" s="271" t="inlineStr">
-        <is>
-          <t>nan nan, nan - nan</t>
-        </is>
-      </c>
-      <c r="L6" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M6" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N6" s="281" t="n">
-        <v>-34.55602</v>
-      </c>
-      <c r="O6" s="283" t="n">
-        <v>-58.41298</v>
-      </c>
-      <c r="P6" s="284" t="inlineStr">
-        <is>
-          <t>07/10/2024</t>
-        </is>
-      </c>
-      <c r="Q6" s="286" t="inlineStr">
-        <is>
-          <t>22:20</t>
-        </is>
-      </c>
-      <c r="R6" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S6" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T6" t="n">
-        <v/>
-      </c>
+      <c r="B6" s="270" t="n"/>
+      <c r="C6" s="277" t="n"/>
+      <c r="D6" s="271" t="n"/>
+      <c r="E6" s="272" t="n"/>
+      <c r="F6" s="272" t="n"/>
+      <c r="G6" s="272" t="n"/>
+      <c r="H6" s="272" t="n"/>
+      <c r="I6" s="307" t="n"/>
+      <c r="J6" s="269" t="n"/>
+      <c r="K6" s="271" t="n"/>
+      <c r="L6" s="265" t="n"/>
+      <c r="M6" s="265" t="n"/>
+      <c r="N6" s="281" t="n"/>
+      <c r="O6" s="283" t="n"/>
+      <c r="P6" s="284" t="n"/>
+      <c r="Q6" s="286" t="n"/>
+      <c r="R6" s="274" t="n"/>
+      <c r="S6" s="275" t="n"/>
       <c r="Y6" s="305" t="n"/>
       <c r="Z6" s="305" t="n"/>
     </row>
     <row r="7" ht="18.75" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B7" s="277" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C7" s="277" t="inlineStr">
-        <is>
-          <t>PS-0575-AER/24</t>
-        </is>
-      </c>
-      <c r="D7" s="272" t="inlineStr">
-        <is>
-          <t>PS-0575-AER/24-(2)</t>
-        </is>
-      </c>
-      <c r="E7" s="272" t="inlineStr">
-        <is>
-          <t>AER</t>
-        </is>
-      </c>
-      <c r="F7" s="272" t="inlineStr">
-        <is>
-          <t>DENUNCIA POLICIAL</t>
-        </is>
-      </c>
-      <c r="G7" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN POLICIAL</t>
-        </is>
-      </c>
-      <c r="H7" s="272" t="inlineStr">
-        <is>
-          <t>CIUDAD AUTONOMA DE BUENOS AIRES</t>
-        </is>
-      </c>
-      <c r="I7" s="307" t="inlineStr">
-        <is>
-          <t>COMUNA 14</t>
-        </is>
-      </c>
-      <c r="J7" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K7" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L7" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M7" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N7" s="280" t="n">
-        <v>-34.5580305</v>
-      </c>
-      <c r="O7" s="282" t="n">
-        <v>-58.4191975</v>
-      </c>
-      <c r="P7" s="284" t="inlineStr">
-        <is>
-          <t>13/10/2024</t>
-        </is>
-      </c>
-      <c r="Q7" s="286" t="inlineStr">
-        <is>
-          <t>05:30</t>
-        </is>
-      </c>
-      <c r="R7" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S7" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T7" t="n">
-        <v/>
-      </c>
+      <c r="B7" s="277" t="n"/>
+      <c r="C7" s="277" t="n"/>
+      <c r="D7" s="272" t="n"/>
+      <c r="E7" s="272" t="n"/>
+      <c r="F7" s="272" t="n"/>
+      <c r="G7" s="272" t="n"/>
+      <c r="H7" s="272" t="n"/>
+      <c r="I7" s="307" t="n"/>
+      <c r="J7" s="272" t="n"/>
+      <c r="K7" s="272" t="n"/>
+      <c r="L7" s="265" t="n"/>
+      <c r="M7" s="265" t="n"/>
+      <c r="N7" s="280" t="n"/>
+      <c r="O7" s="282" t="n"/>
+      <c r="P7" s="284" t="n"/>
+      <c r="Q7" s="286" t="n"/>
+      <c r="R7" s="274" t="n"/>
+      <c r="S7" s="275" t="n"/>
       <c r="Y7" s="305" t="n"/>
       <c r="Z7" s="305" t="n"/>
     </row>
     <row r="8" ht="18.75" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B8" s="277" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C8" s="277" t="inlineStr">
-        <is>
-          <t>ACTUACIONES JUDICIALES-0000-UC1/24</t>
-        </is>
-      </c>
-      <c r="D8" s="272" t="inlineStr">
-        <is>
-          <t>ACTUACIONES JUDICIALES-0000-UC1/24-(1)</t>
-        </is>
-      </c>
-      <c r="E8" s="272" t="inlineStr">
-        <is>
-          <t>UC1</t>
-        </is>
-      </c>
-      <c r="F8" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN DE ALLANAMIENTO</t>
-        </is>
-      </c>
-      <c r="G8" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN JUDICIAL</t>
-        </is>
-      </c>
-      <c r="H8" s="272" t="inlineStr">
-        <is>
-          <t>CIUDAD AUTONOMA DE BUENOS AIRES</t>
-        </is>
-      </c>
-      <c r="I8" s="307" t="inlineStr">
-        <is>
-          <t>UC1</t>
-        </is>
-      </c>
-      <c r="J8" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K8" s="272" t="inlineStr">
-        <is>
-          <t>GENERAL CESAR DIAZ 4342, nan - nan</t>
-        </is>
-      </c>
-      <c r="L8" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M8" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N8" s="280" t="n">
-        <v>-34.6242611</v>
-      </c>
-      <c r="O8" s="282" t="n">
-        <v>-58.4932984</v>
-      </c>
-      <c r="P8" s="284" t="inlineStr">
-        <is>
-          <t>18/10/2024</t>
-        </is>
-      </c>
-      <c r="Q8" s="286" t="inlineStr">
-        <is>
-          <t>07:36</t>
-        </is>
-      </c>
-      <c r="R8" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S8" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T8" t="n">
-        <v/>
-      </c>
+      <c r="B8" s="277" t="n"/>
+      <c r="C8" s="277" t="n"/>
+      <c r="D8" s="272" t="n"/>
+      <c r="E8" s="272" t="n"/>
+      <c r="F8" s="272" t="n"/>
+      <c r="G8" s="272" t="n"/>
+      <c r="H8" s="272" t="n"/>
+      <c r="I8" s="307" t="n"/>
+      <c r="J8" s="272" t="n"/>
+      <c r="K8" s="272" t="n"/>
+      <c r="L8" s="265" t="n"/>
+      <c r="M8" s="265" t="n"/>
+      <c r="N8" s="280" t="n"/>
+      <c r="O8" s="282" t="n"/>
+      <c r="P8" s="284" t="n"/>
+      <c r="Q8" s="286" t="n"/>
+      <c r="R8" s="274" t="n"/>
+      <c r="S8" s="275" t="n"/>
       <c r="Y8" s="305" t="n"/>
       <c r="Z8" s="305" t="n"/>
     </row>
     <row r="9" ht="18" customHeight="1" s="261" thickBot="1">
-      <c r="B9" s="277" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C9" s="277" t="inlineStr">
-        <is>
-          <t>FCB-14653/24 COIRON-222549/24</t>
-        </is>
-      </c>
-      <c r="D9" s="272" t="inlineStr">
-        <is>
-          <t>FCB-14653/24 COIRON-222549/24-(1)</t>
-        </is>
-      </c>
-      <c r="E9" s="272" t="inlineStr">
-        <is>
-          <t>UC2</t>
-        </is>
-      </c>
-      <c r="F9" s="272" t="inlineStr">
-        <is>
-          <t>DENUNCIA POLICIAL</t>
-        </is>
-      </c>
-      <c r="G9" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN POLICIAL</t>
-        </is>
-      </c>
-      <c r="H9" s="272" t="inlineStr">
-        <is>
-          <t>CORDOBA</t>
-        </is>
-      </c>
-      <c r="I9" s="307" t="inlineStr">
-        <is>
-          <t>UC2</t>
-        </is>
-      </c>
-      <c r="J9" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K9" s="272" t="inlineStr">
-        <is>
-          <t>EDUARDO MARQUINA S/D, CORDOBA - nan</t>
-        </is>
-      </c>
-      <c r="L9" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M9" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N9" s="280" t="n">
-        <v>-31.381514</v>
-      </c>
-      <c r="O9" s="282" t="n">
-        <v>-64.192876</v>
-      </c>
-      <c r="P9" s="284" t="inlineStr">
-        <is>
-          <t>14/10/2024</t>
-        </is>
-      </c>
-      <c r="Q9" s="286" t="inlineStr">
-        <is>
-          <t>12:36</t>
-        </is>
-      </c>
-      <c r="R9" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S9" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T9" t="n">
-        <v/>
-      </c>
+      <c r="B9" s="277" t="n"/>
+      <c r="C9" s="277" t="n"/>
+      <c r="D9" s="272" t="n"/>
+      <c r="E9" s="272" t="n"/>
+      <c r="F9" s="272" t="n"/>
+      <c r="G9" s="272" t="n"/>
+      <c r="H9" s="272" t="n"/>
+      <c r="I9" s="307" t="n"/>
+      <c r="J9" s="272" t="n"/>
+      <c r="K9" s="272" t="n"/>
+      <c r="L9" s="265" t="n"/>
+      <c r="M9" s="265" t="n"/>
+      <c r="N9" s="280" t="n"/>
+      <c r="O9" s="282" t="n"/>
+      <c r="P9" s="284" t="n"/>
+      <c r="Q9" s="286" t="n"/>
+      <c r="R9" s="274" t="n"/>
+      <c r="S9" s="275" t="n"/>
       <c r="Y9" s="305" t="n"/>
       <c r="Z9" s="305" t="n"/>
     </row>
     <row r="10" ht="18.75" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B10" s="277" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C10" s="277" t="inlineStr">
-        <is>
-          <t>179/2023 (8178)</t>
-        </is>
-      </c>
-      <c r="D10" s="272" t="inlineStr">
-        <is>
-          <t>179/2023 (8178)-(1)</t>
-        </is>
-      </c>
-      <c r="E10" s="272" t="inlineStr">
-        <is>
-          <t>AER</t>
-        </is>
-      </c>
-      <c r="F10" s="272" t="inlineStr">
-        <is>
-          <t>DENUNCIA POLICIAL</t>
-        </is>
-      </c>
-      <c r="G10" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN POLICIAL</t>
-        </is>
-      </c>
-      <c r="H10" s="272" t="inlineStr">
-        <is>
-          <t>CIUDAD AUTONOMA DE BUENOS AIRES</t>
-        </is>
-      </c>
-      <c r="I10" s="307" t="inlineStr">
-        <is>
-          <t>COMUNA 14</t>
-        </is>
-      </c>
-      <c r="J10" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K10" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L10" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M10" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N10" s="278" t="n">
-        <v>-34.5580305</v>
-      </c>
-      <c r="O10" s="282" t="n">
-        <v>-58.4191975</v>
-      </c>
-      <c r="P10" s="284" t="inlineStr">
-        <is>
-          <t>19/10/2024</t>
-        </is>
-      </c>
-      <c r="Q10" s="286" t="inlineStr">
-        <is>
-          <t>08:20</t>
-        </is>
-      </c>
-      <c r="R10" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S10" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T10" t="n">
-        <v/>
-      </c>
+      <c r="B10" s="277" t="n"/>
+      <c r="C10" s="277" t="n"/>
+      <c r="D10" s="272" t="n"/>
+      <c r="E10" s="272" t="n"/>
+      <c r="F10" s="272" t="n"/>
+      <c r="G10" s="272" t="n"/>
+      <c r="H10" s="272" t="n"/>
+      <c r="I10" s="307" t="n"/>
+      <c r="J10" s="272" t="n"/>
+      <c r="K10" s="272" t="n"/>
+      <c r="L10" s="265" t="n"/>
+      <c r="M10" s="265" t="n"/>
+      <c r="N10" s="278" t="n"/>
+      <c r="O10" s="282" t="n"/>
+      <c r="P10" s="284" t="n"/>
+      <c r="Q10" s="286" t="n"/>
+      <c r="R10" s="274" t="n"/>
+      <c r="S10" s="275" t="n"/>
       <c r="Y10" s="305" t="n"/>
       <c r="Z10" s="305" t="n"/>
     </row>
     <row r="11" ht="18" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B11" s="277" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C11" s="277" t="inlineStr">
-        <is>
-          <t>42933 "M" 2021</t>
-        </is>
-      </c>
-      <c r="D11" s="269" t="inlineStr">
-        <is>
-          <t>42933 "M" 2021-(1)</t>
-        </is>
-      </c>
-      <c r="E11" s="269" t="inlineStr">
-        <is>
-          <t>COR</t>
-        </is>
-      </c>
-      <c r="F11" s="269" t="inlineStr">
-        <is>
-          <t>DENUNCIA POLICIAL</t>
-        </is>
-      </c>
-      <c r="G11" s="269" t="inlineStr">
-        <is>
-          <t>ORDEN POLICIAL</t>
-        </is>
-      </c>
-      <c r="H11" s="272" t="inlineStr">
-        <is>
-          <t>CORDOBA</t>
-        </is>
-      </c>
-      <c r="I11" s="307" t="inlineStr">
-        <is>
-          <t>CAPITAL</t>
-        </is>
-      </c>
-      <c r="J11" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K11" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L11" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M11" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N11" s="279" t="n">
-        <v>-31.315538</v>
-      </c>
-      <c r="O11" s="279" t="n">
-        <v>-64.213374</v>
-      </c>
-      <c r="P11" s="284" t="inlineStr">
-        <is>
-          <t>20/10/2024</t>
-        </is>
-      </c>
-      <c r="Q11" s="287" t="inlineStr">
-        <is>
-          <t>03:30</t>
-        </is>
-      </c>
-      <c r="R11" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S11" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T11" t="n">
-        <v/>
-      </c>
+      <c r="B11" s="277" t="n"/>
+      <c r="C11" s="277" t="n"/>
+      <c r="D11" s="269" t="n"/>
+      <c r="E11" s="269" t="n"/>
+      <c r="F11" s="269" t="n"/>
+      <c r="G11" s="269" t="n"/>
+      <c r="H11" s="272" t="n"/>
+      <c r="I11" s="307" t="n"/>
+      <c r="J11" s="272" t="n"/>
+      <c r="K11" s="272" t="n"/>
+      <c r="L11" s="265" t="n"/>
+      <c r="M11" s="265" t="n"/>
+      <c r="N11" s="279" t="n"/>
+      <c r="O11" s="279" t="n"/>
+      <c r="P11" s="284" t="n"/>
+      <c r="Q11" s="287" t="n"/>
+      <c r="R11" s="274" t="n"/>
+      <c r="S11" s="275" t="n"/>
       <c r="Y11" s="305" t="n"/>
       <c r="Z11" s="305" t="n"/>
     </row>
     <row r="12" ht="22.5" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B12" s="277" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C12" s="277" t="inlineStr">
-        <is>
-          <t>27091/2022</t>
-        </is>
-      </c>
-      <c r="D12" s="272" t="inlineStr">
-        <is>
-          <t>27091/2022-(1)</t>
-        </is>
-      </c>
-      <c r="E12" s="272" t="inlineStr">
-        <is>
-          <t>UCC</t>
-        </is>
-      </c>
-      <c r="F12" s="269" t="inlineStr">
-        <is>
-          <t>ORDEN DE ALLANAMIENTO</t>
-        </is>
-      </c>
-      <c r="G12" s="269" t="inlineStr">
-        <is>
-          <t>ORDEN JUDICIAL</t>
-        </is>
-      </c>
-      <c r="H12" s="272" t="inlineStr">
-        <is>
-          <t>BUENOS AIRES</t>
-        </is>
-      </c>
-      <c r="I12" s="307" t="inlineStr">
-        <is>
-          <t>UCC</t>
-        </is>
-      </c>
-      <c r="J12" s="272" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K12" s="276" t="inlineStr">
-        <is>
-          <t>VILLEGAS 149, EL PALOMAR - MORON</t>
-        </is>
-      </c>
-      <c r="L12" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M12" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N12" s="264" t="n">
-        <v>-34.623564</v>
-      </c>
-      <c r="O12" s="262" t="n">
-        <v>-58.577936</v>
-      </c>
-      <c r="P12" s="263" t="inlineStr">
-        <is>
-          <t>22/10/2024</t>
-        </is>
-      </c>
-      <c r="Q12" s="285" t="inlineStr">
-        <is>
-          <t>07:57</t>
-        </is>
-      </c>
-      <c r="R12" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S12" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T12" t="n">
-        <v/>
-      </c>
+      <c r="B12" s="277" t="n"/>
+      <c r="C12" s="277" t="n"/>
+      <c r="D12" s="272" t="n"/>
+      <c r="E12" s="272" t="n"/>
+      <c r="F12" s="269" t="n"/>
+      <c r="G12" s="269" t="n"/>
+      <c r="H12" s="272" t="n"/>
+      <c r="I12" s="307" t="n"/>
+      <c r="J12" s="272" t="n"/>
+      <c r="K12" s="276" t="n"/>
+      <c r="L12" s="265" t="n"/>
+      <c r="M12" s="265" t="n"/>
+      <c r="N12" s="264" t="n"/>
+      <c r="O12" s="262" t="n"/>
+      <c r="P12" s="263" t="n"/>
+      <c r="Q12" s="285" t="n"/>
+      <c r="R12" s="274" t="n"/>
+      <c r="S12" s="275" t="n"/>
       <c r="Y12" s="305" t="n"/>
       <c r="Z12" s="305" t="n"/>
     </row>
     <row r="13" ht="22.5" customFormat="1" customHeight="1" s="313" thickBot="1">
-      <c r="B13" s="270" t="inlineStr">
-        <is>
-          <t>PSA</t>
-        </is>
-      </c>
-      <c r="C13" s="277" t="inlineStr">
-        <is>
-          <t>27091/2022</t>
-        </is>
-      </c>
-      <c r="D13" s="271" t="inlineStr">
-        <is>
-          <t>27091/2022-(2)</t>
-        </is>
-      </c>
-      <c r="E13" s="272" t="inlineStr">
-        <is>
-          <t>UCC</t>
-        </is>
-      </c>
-      <c r="F13" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN DE ALLANAMIENTO</t>
-        </is>
-      </c>
-      <c r="G13" s="272" t="inlineStr">
-        <is>
-          <t>ORDEN JUDICIAL</t>
-        </is>
-      </c>
-      <c r="H13" s="272" t="inlineStr">
-        <is>
-          <t>BUENOS AIRES</t>
-        </is>
-      </c>
-      <c r="I13" s="307" t="inlineStr">
-        <is>
-          <t>UCC</t>
-        </is>
-      </c>
-      <c r="J13" s="269" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K13" s="271" t="inlineStr">
-        <is>
-          <t>BELGRANO 6564, JOSE LEON SUAREZ - SAN MARTIN</t>
-        </is>
-      </c>
-      <c r="L13" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M13" s="265" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N13" s="281" t="n">
-        <v>-34.541669</v>
-      </c>
-      <c r="O13" s="283" t="n">
-        <v>-58.574293</v>
-      </c>
-      <c r="P13" s="263" t="inlineStr">
-        <is>
-          <t>22/10/2024</t>
-        </is>
-      </c>
-      <c r="Q13" s="286" t="inlineStr">
-        <is>
-          <t>07:40</t>
-        </is>
-      </c>
-      <c r="R13" s="274" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S13" s="275" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T13" t="n">
-        <v/>
-      </c>
+      <c r="B13" s="270" t="n"/>
+      <c r="C13" s="277" t="n"/>
+      <c r="D13" s="271" t="n"/>
+      <c r="E13" s="272" t="n"/>
+      <c r="F13" s="272" t="n"/>
+      <c r="G13" s="272" t="n"/>
+      <c r="H13" s="272" t="n"/>
+      <c r="I13" s="307" t="n"/>
+      <c r="J13" s="269" t="n"/>
+      <c r="K13" s="271" t="n"/>
+      <c r="L13" s="265" t="n"/>
+      <c r="M13" s="265" t="n"/>
+      <c r="N13" s="281" t="n"/>
+      <c r="O13" s="283" t="n"/>
+      <c r="P13" s="263" t="n"/>
+      <c r="Q13" s="286" t="n"/>
+      <c r="R13" s="274" t="n"/>
+      <c r="S13" s="275" t="n"/>
       <c r="Y13" s="305" t="n"/>
       <c r="Z13" s="305" t="n"/>
     </row>
@@ -21435,7 +20725,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -24823,7 +24113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -30487,13 +29777,13 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -35385,13 +34675,13 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -35559,13 +34849,13 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -35711,13 +35001,13 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -36386,13 +35676,13 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -36515,7 +35805,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="598"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>